<commit_message>
v1 of output testing
</commit_message>
<xml_diff>
--- a/src/main/resources/assignments-config.xlsx
+++ b/src/main/resources/assignments-config.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="A4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>C</t>
   </si>
@@ -40,6 +41,36 @@
   </si>
   <si>
     <t>Test Format</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>5x3</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>6/2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>basic</t>
   </si>
 </sst>
 </file>
@@ -88,7 +119,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -96,17 +127,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,87 +482,169 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
output testing runthrough 1, c is a bit strange though
</commit_message>
<xml_diff>
--- a/src/main/resources/assignments-config.xlsx
+++ b/src/main/resources/assignments-config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,8 +123,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -144,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -152,6 +154,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -159,6 +162,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -591,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Some modifications for actual server
</commit_message>
<xml_diff>
--- a/src/main/resources/assignments-config.xlsx
+++ b/src/main/resources/assignments-config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>C</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>6 2 /</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Counting occurrences of letters</t>
+  </si>
+  <si>
+    <t>C implementation of infix to postfix</t>
+  </si>
+  <si>
+    <t>Java implementation of infix to postfix</t>
+  </si>
+  <si>
+    <t>Calculator output</t>
   </si>
 </sst>
 </file>
@@ -123,8 +138,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -152,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -164,6 +191,12 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -175,6 +208,12 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -515,7 +554,7 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -525,8 +564,11 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -536,8 +578,11 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -547,8 +592,11 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -558,8 +606,11 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -568,6 +619,9 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>